<commit_message>
Added test case for "Multiple Users"
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint2.xlsx
+++ b/Test-cases/Sprint2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User unique views" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Purpose :</t>
   </si>
@@ -51,21 +51,12 @@
     <t>MM/DD/YYYY</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Blank</t>
   </si>
   <si>
     <t>Not Tested</t>
   </si>
   <si>
-    <t>"The order has been delivered" message is displayed. The order no longer appears in the order list.</t>
-  </si>
-  <si>
-    <t>"Confirmation is sent to the customer and the order has been delivered" message is displayed.  The order no longer appears in the order list.</t>
-  </si>
-  <si>
     <t>Test103</t>
   </si>
   <si>
@@ -109,6 +100,45 @@
   </si>
   <si>
     <t>Valid</t>
+  </si>
+  <si>
+    <t>"The username field is required" message is displayed.</t>
+  </si>
+  <si>
+    <t>"The password field is required" message is displayed.</t>
+  </si>
+  <si>
+    <t>Should login with the username and display application home page.</t>
+  </si>
+  <si>
+    <t>Verify multiple users are supported by the application.</t>
+  </si>
+  <si>
+    <t>Customers can access the website.</t>
+  </si>
+  <si>
+    <t>1. Open the applcation in different browsers.</t>
+  </si>
+  <si>
+    <t>2. click on login</t>
+  </si>
+  <si>
+    <t>3. Enter valid username,password.</t>
+  </si>
+  <si>
+    <t>4. Click Login</t>
+  </si>
+  <si>
+    <t>Expected:</t>
+  </si>
+  <si>
+    <t>All the users are able to login and access the site</t>
+  </si>
+  <si>
+    <t>Test Result :</t>
+  </si>
+  <si>
+    <t>Test104</t>
   </si>
 </sst>
 </file>
@@ -255,7 +285,119 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -919,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -937,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -953,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -966,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -983,7 +1125,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -991,7 +1133,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -999,7 +1141,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -1007,7 +1149,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -1024,10 +1166,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>5</v>
@@ -1051,71 +1193,73 @@
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="F17" s="11"/>
     </row>
@@ -1134,46 +1278,46 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1189,12 +1333,187 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added test case for "Manager can add items and prices"
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint2.xlsx
+++ b/Test-cases/Sprint2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="User unique views" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
   <si>
     <t>Purpose :</t>
   </si>
@@ -139,6 +139,72 @@
   </si>
   <si>
     <t>Test104</t>
+  </si>
+  <si>
+    <t>Test106</t>
+  </si>
+  <si>
+    <t>Verify manager can add items and prices.</t>
+  </si>
+  <si>
+    <t>Manager is logged in.</t>
+  </si>
+  <si>
+    <t>1. Click on menu/Manager(Now change it later)</t>
+  </si>
+  <si>
+    <t>2. Application displays a list of items.</t>
+  </si>
+  <si>
+    <t>3. Click on add new</t>
+  </si>
+  <si>
+    <t>4. Application displays a form to be filled</t>
+  </si>
+  <si>
+    <t>5. Fill the form</t>
+  </si>
+  <si>
+    <t>6. Click create.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test106.A</t>
+  </si>
+  <si>
+    <t>Test106.B</t>
+  </si>
+  <si>
+    <t>Test106.C</t>
+  </si>
+  <si>
+    <t>Test106.D</t>
+  </si>
+  <si>
+    <t>Test106.E</t>
+  </si>
+  <si>
+    <t>Test106.F</t>
+  </si>
+  <si>
+    <t>"The name field is required"  and "The price field is required"message is displayed.</t>
+  </si>
+  <si>
+    <t>"The name field is required"  message is displayed.</t>
+  </si>
+  <si>
+    <t>"The price field is required"  message is displayed.</t>
+  </si>
+  <si>
+    <t>Displays the list of items in menu with the new item added in it.</t>
   </si>
 </sst>
 </file>
@@ -209,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -232,13 +298,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -279,13 +371,806 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="154">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1278,46 +2163,46 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="41" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1335,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1465,46 +2350,46 @@
     <mergeCell ref="C3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1532,13 +2417,440 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F16:F18 F21">
+    <cfRule type="cellIs" dxfId="41" priority="43" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="44" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="45" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="46" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="47" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="48" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="49" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="50" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="51" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="52" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="53" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="54" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="55" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="56" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="cellIs" dxfId="27" priority="29" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="31" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="32" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="33" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="34" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="35" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="36" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="37" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="38" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="39" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="40" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="41" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="42" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="13" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="25" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="28" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F21">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added test case " Managers can edit/delete menu items"
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint2.xlsx
+++ b/Test-cases/Sprint2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="User unique views" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
   <si>
     <t>Purpose :</t>
   </si>
@@ -205,6 +205,40 @@
   </si>
   <si>
     <t>Displays the list of items in menu with the new item added in it.</t>
+  </si>
+  <si>
+    <t>Test107</t>
+  </si>
+  <si>
+    <t>Verify manager can edit/delete items and prices.</t>
+  </si>
+  <si>
+    <t>4. Application displays a form with items.</t>
+  </si>
+  <si>
+    <t>5. Make change to the form</t>
+  </si>
+  <si>
+    <t>6. Click save.</t>
+  </si>
+  <si>
+    <t>Steps 1:</t>
+  </si>
+  <si>
+    <t>Steps 2:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Click on edit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Click on delete </t>
+  </si>
+  <si>
+    <t>3. Select the items to be deleted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Edited items should get displayed in the menu list.    
+2. Deleted items are not displayed in the menu list.                              </t>
   </si>
 </sst>
 </file>
@@ -386,7 +420,231 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="154">
+  <dxfs count="182">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2163,46 +2421,46 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="69" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2221,7 +2479,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2350,46 +2608,46 @@
     <mergeCell ref="C3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2419,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2712,134 +2970,134 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F16:F18 F21">
-    <cfRule type="cellIs" dxfId="41" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="43" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="45" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="46" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="47" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="48" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="49" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="50" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="51" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="52" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="54" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="55" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="27" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="38" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="39" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="13" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="15" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="19" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="23" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2856,12 +3114,248 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added test case for "User unique views"
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint2.xlsx
+++ b/Test-cases/Sprint2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="User unique views" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Employee confirm order" sheetId="8" r:id="rId8"/>
     <sheet name="Employee confirm delivery" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
   <si>
     <t>Purpose :</t>
   </si>
@@ -239,6 +239,84 @@
   <si>
     <t xml:space="preserve">1. Edited items should get displayed in the menu list.    
 2. Deleted items are not displayed in the menu list.                              </t>
+  </si>
+  <si>
+    <t>Verify different user types have all the necessary views.</t>
+  </si>
+  <si>
+    <t>1. Click on Login</t>
+  </si>
+  <si>
+    <t>2. Type in user name and password</t>
+  </si>
+  <si>
+    <t>3. Clik on Login</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Test101</t>
+  </si>
+  <si>
+    <t>Test101.A</t>
+  </si>
+  <si>
+    <t>Test101.B</t>
+  </si>
+  <si>
+    <t>Test101.C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager </t>
+  </si>
+  <si>
+    <t>Must be able to do the following:</t>
+  </si>
+  <si>
+    <t>1. Can view menu</t>
+  </si>
+  <si>
+    <t>2. Can place order</t>
+  </si>
+  <si>
+    <t>3. Can monitor order</t>
+  </si>
+  <si>
+    <t>4. Can view history.</t>
+  </si>
+  <si>
+    <t>5. Can edit personal information.</t>
+  </si>
+  <si>
+    <t>2. Can view order</t>
+  </si>
+  <si>
+    <t>3. Can confirm order</t>
+  </si>
+  <si>
+    <t>4. Can confirm deliver.</t>
+  </si>
+  <si>
+    <t>5. Can view customer info.</t>
+  </si>
+  <si>
+    <t>6. Can view customer order history</t>
+  </si>
+  <si>
+    <t>7. Can block customer.</t>
+  </si>
+  <si>
+    <t>8. Can add/edit/delete menu items and prices.</t>
   </si>
 </sst>
 </file>
@@ -364,7 +442,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -414,13 +492,352 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="182">
+  <dxfs count="224">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="50"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="22"/>
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="26"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="44"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2174,14 +2591,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F13 F30 F20">
+    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Partially Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Partially Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13 F20 F30">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2191,7 +2955,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2421,46 +3185,46 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2608,46 +3372,46 @@
     <mergeCell ref="C3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="83" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2970,134 +3734,134 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="F16:F18 F21">
-    <cfRule type="cellIs" dxfId="69" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="43" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="44" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="45" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="46" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="47" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="48" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="51" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="52" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="53" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="54" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="55" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="56" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="55" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="29" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="30" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="32" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="37" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="38" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="39" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="41" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="42" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="41" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="15" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="16" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="18" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="28" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3116,8 +3880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3307,46 +4071,46 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Partially Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Partially Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3376,7 +4140,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Tested Sprint 2 in Mozilla
</commit_message>
<xml_diff>
--- a/Test-cases/Sprint2.xlsx
+++ b/Test-cases/Sprint2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26840" windowHeight="16080" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="User unique views" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="130">
   <si>
     <t>Purpose :</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Test Result</t>
-  </si>
-  <si>
-    <t>Remarks</t>
   </si>
   <si>
     <t>MM/DD/YYYY</t>
@@ -348,9 +345,6 @@
     <t>New/Updated personal informaiton should be displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve"> NOT OK</t>
-  </si>
-  <si>
     <t>Test201</t>
   </si>
   <si>
@@ -409,6 +403,23 @@
   </si>
   <si>
     <t xml:space="preserve">1. A new employee account is created.                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Remarks(chrome)
+</t>
+  </si>
+  <si>
+    <t>Remarks(Mozilla)</t>
+  </si>
+  <si>
+    <t>Remarks(chrome)</t>
+  </si>
+  <si>
+    <t>1. Tested(Chrome)</t>
+  </si>
+  <si>
+    <t>2. Tested(Mozilla)</t>
   </si>
 </sst>
 </file>
@@ -573,7 +584,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -638,11 +649,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1082,35 +1096,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1118,12 +1133,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1131,16 +1146,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1148,27 +1163,27 @@
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:7" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:7" ht="12.75" customHeight="1">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:7" ht="12.75" customHeight="1">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -1176,338 +1191,406 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="24"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="E18" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>97</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>97</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="15" t="s">
-        <v>97</v>
-      </c>
       <c r="G28" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>97</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>97</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7">
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="5:7">
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="5:7">
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="5:7">
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="5:7">
-      <c r="E37" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="F37" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="5:7">
+        <v>97</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
+  <mergeCells count="12">
+    <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="F13 F30 F20">
     <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
@@ -1570,35 +1653,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="22" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1606,12 +1689,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1619,16 +1702,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1636,35 +1719,35 @@
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -1672,132 +1755,149 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="24">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
+      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2" t="s">
+      <c r="E16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="24">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="E17" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>97</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1810,36 +1910,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="10.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="21" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1847,13 +1947,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1861,60 +1961,60 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1922,32 +2022,49 @@
         <v>5</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D12" s="23"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>98</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C16" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1960,35 +2077,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:XFD1048576"/>
+      <selection activeCell="C12" sqref="C12:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1996,12 +2113,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2009,16 +2126,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -2026,62 +2143,70 @@
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="63.75" customHeight="1">
+    <row r="11" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" s="23"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>98</v>
+        <v>35</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C13" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2105,36 +2230,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="20" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="20" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="20" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="20"/>
+    <col min="1" max="1" width="10.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="16" style="20" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="20" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="20" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2142,13 +2267,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2156,68 +2281,68 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -2225,28 +2350,36 @@
         <v>5</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D13" s="23"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D14" s="23"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>98</v>
+        <v>35</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C17" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2271,35 +2404,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="16" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5" style="16" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="16"/>
+    <col min="1" max="1" width="10.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2307,12 +2440,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2320,16 +2453,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -2337,62 +2470,70 @@
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="63.75" customHeight="1">
+    <row r="11" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="23"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>106</v>
+        <v>35</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C13" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2416,36 +2557,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H14" sqref="H14:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2453,12 +2594,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2466,16 +2607,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -2483,49 +2624,49 @@
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -2533,190 +2674,213 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="25" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="17"/>
-      <c r="G14" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="25"/>
+      <c r="G14" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="1:7" ht="24">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="F18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="24">
-      <c r="A19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="24">
-      <c r="A21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2729,36 +2893,36 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:D18"/>
+      <selection activeCell="C20" sqref="C20:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="51.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2766,13 +2930,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2780,110 +2944,110 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:6" ht="38.25" customHeight="1">
+    <row r="10" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="23"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="23"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="23"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="23"/>
     </row>
-    <row r="16" spans="1:6" ht="25.5" customHeight="1">
+    <row r="16" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="51" customHeight="1">
+    <row r="18" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -2891,22 +3055,30 @@
         <v>5</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="23"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>97</v>
+        <v>35</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2937,18 +3109,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="20"/>
@@ -2956,7 +3129,7 @@
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="20"/>
@@ -2964,7 +3137,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2972,13 +3145,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" ht="24">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2986,23 +3159,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="20"/>
@@ -3010,51 +3183,51 @@
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="20"/>
@@ -3062,7 +3235,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="20"/>
@@ -3070,7 +3243,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -3078,23 +3251,23 @@
         <v>5</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
@@ -3102,31 +3275,35 @@
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="1:6" ht="24">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>98</v>
+        <v>35</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>97</v>
+      </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>

</xml_diff>